<commit_message>
hardware: outputs: Updating outputs for IIP Nº3 board #65
</commit_message>
<xml_diff>
--- a/hardware/outputs/board_bom/board_bom_iip_quad_uart.xlsx
+++ b/hardware/outputs/board_bom/board_bom_iip_quad_uart.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yan Azeredo\Desktop\SpaceLab\interface-board\semi_usb_interface\outputs\board_bom\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C101E69-D006-429A-B0E1-5F105CE4D4B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C36F74DC-DDC4-4DD6-A693-F20C5445D588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -38,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
   <si>
     <t>Source Data From:</t>
   </si>
@@ -73,10 +68,10 @@
     <t>IIPN3</t>
   </si>
   <si>
-    <t>11/29/2020</t>
-  </si>
-  <si>
-    <t>11:31 PM</t>
+    <t>7/1/2021</t>
+  </si>
+  <si>
+    <t>12:09:42 AM</t>
   </si>
   <si>
     <t>Designator</t>
@@ -127,43 +122,7 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>Wurth Electronics</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
-    <t>Kyocera AVX</t>
-  </si>
-  <si>
-    <t>Molex</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>Yageo</t>
-  </si>
-  <si>
-    <t>TXC</t>
-  </si>
-  <si>
-    <t>Vishay</t>
-  </si>
-  <si>
-    <t>FTDI</t>
-  </si>
-  <si>
-    <t>Stackpole Electronics</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
+    <t>#Column Name Error:Manufacturer</t>
   </si>
   <si>
     <t>Manufacturer Part Number</t>
@@ -175,6 +134,9 @@
     <t>C2012X7R1E475K125AB</t>
   </si>
   <si>
+    <t>742792608</t>
+  </si>
+  <si>
     <t>CRCW080510K0FKEA</t>
   </si>
   <si>
@@ -190,6 +152,9 @@
     <t>RC0603FR-0710RL</t>
   </si>
   <si>
+    <t>651005136421</t>
+  </si>
+  <si>
     <t>AA-12.000MAGE-T</t>
   </si>
   <si>
@@ -205,7 +170,7 @@
     <t>TPS79333DBVR</t>
   </si>
   <si>
-    <t>#Column Name Error:' Partnumber</t>
+    <t>#Column Name Error:Partnumber</t>
   </si>
   <si>
     <t>Description</t>
@@ -253,49 +218,13 @@
     <t>TEXAS INSTRUMENTS - TPS79333DBVR - IC, V REG, LINEAR, 0.2A, SOT-23-5</t>
   </si>
   <si>
-    <t>#Column Name Error:' Package</t>
-  </si>
-  <si>
-    <t>Footprint</t>
-  </si>
-  <si>
-    <t>C0603_MD</t>
-  </si>
-  <si>
-    <t>C0805_MD</t>
-  </si>
-  <si>
-    <t>L0603</t>
-  </si>
-  <si>
-    <t>R0805_MD</t>
-  </si>
-  <si>
-    <t>PICO BLADE 0533980571</t>
-  </si>
-  <si>
-    <t>R0603_MD</t>
-  </si>
-  <si>
-    <t>MINI USB B 180GRAUS WE</t>
-  </si>
-  <si>
-    <t>TXC 7A Series</t>
-  </si>
-  <si>
-    <t>LQFP-64</t>
-  </si>
-  <si>
-    <t>SOT23-5</t>
-  </si>
-  <si>
-    <t>Mount</t>
-  </si>
-  <si>
-    <t>Surface Mount</t>
-  </si>
-  <si>
-    <t>Through Hole,Vertical</t>
+    <t>#Column Name Error:Package</t>
+  </si>
+  <si>
+    <t>#Column Name Error:Footprint</t>
+  </si>
+  <si>
+    <t>#Column Name Error:Mount</t>
   </si>
   <si>
     <t>Fitted</t>
@@ -476,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -539,11 +468,59 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -611,22 +588,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>129541</xdr:rowOff>
+      <xdr:rowOff>191767</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>260858</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>30481</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88991</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="A close up of a logo&#10;&#10;Description automatically generated">
+        <xdr:cNvPr id="4" name="Imagem 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C561B77-A4A6-46D4-8A41-F4ACD0CFFC91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6EA9836-536E-44C0-B283-ED5A8731FF0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -635,7 +612,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -648,8 +625,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7620" y="129541"/>
-          <a:ext cx="2731643" cy="1546860"/>
+          <a:off x="180975" y="191767"/>
+          <a:ext cx="2000250" cy="1402174"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -930,7 +907,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:F5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,11 +1049,11 @@
       </c>
       <c r="E7" s="7">
         <f ca="1">TODAY()</f>
-        <v>44164</v>
+        <v>44378</v>
       </c>
       <c r="F7" s="8">
         <f ca="1">NOW()</f>
-        <v>44164.980396527775</v>
+        <v>44378.006824421296</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -1130,25 +1107,25 @@
         <v>29</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="L10" s="13"/>
     </row>
@@ -1157,31 +1134,25 @@
         <f>ROW(A11) - ROW($A$10)</f>
         <v>1</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="30" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="14">
         <v>14</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>43</v>
+      <c r="D11" s="14"/>
+      <c r="E11" s="30" t="s">
+        <v>31</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="15" t="s">
-        <v>57</v>
+      <c r="G11" s="31" t="s">
+        <v>47</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>86</v>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="51" x14ac:dyDescent="0.25">
@@ -1189,31 +1160,25 @@
         <f t="shared" ref="A12:A24" si="0">ROW(A12) - ROW($A$10)</f>
         <v>2</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="14">
         <v>5</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>44</v>
+      <c r="D12" s="14"/>
+      <c r="E12" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="F12" s="14"/>
-      <c r="G12" s="15" t="s">
-        <v>58</v>
+      <c r="G12" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="H12" s="15"/>
-      <c r="I12" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>86</v>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -1221,31 +1186,25 @@
         <f>ROW(A13) - ROW($A$10)</f>
         <v>3</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="30" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="14">
         <v>3</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="14">
-        <v>742792608</v>
+      <c r="D13" s="14"/>
+      <c r="E13" s="30" t="s">
+        <v>33</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="15" t="s">
-        <v>59</v>
+      <c r="G13" s="31" t="s">
+        <v>49</v>
       </c>
       <c r="H13" s="15"/>
-      <c r="I13" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>86</v>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -1253,29 +1212,25 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="14">
         <v>3</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>45</v>
+      <c r="D14" s="14"/>
+      <c r="E14" s="30" t="s">
+        <v>34</v>
       </c>
       <c r="F14" s="14"/>
-      <c r="G14" s="15" t="s">
-        <v>60</v>
+      <c r="G14" s="31" t="s">
+        <v>50</v>
       </c>
       <c r="H14" s="15"/>
-      <c r="I14" s="15" t="s">
-        <v>76</v>
-      </c>
+      <c r="I14" s="15"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="15" t="s">
-        <v>86</v>
+      <c r="K14" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
@@ -1283,31 +1238,25 @@
         <f>ROW(A15) - ROW($A$10)</f>
         <v>5</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="14">
         <v>2</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>46</v>
+      <c r="D15" s="14"/>
+      <c r="E15" s="30" t="s">
+        <v>35</v>
       </c>
       <c r="F15" s="14"/>
-      <c r="G15" s="15" t="s">
-        <v>61</v>
+      <c r="G15" s="31" t="s">
+        <v>51</v>
       </c>
       <c r="H15" s="15"/>
-      <c r="I15" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>86</v>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.25">
@@ -1315,31 +1264,25 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="14">
         <v>2</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>47</v>
+      <c r="D16" s="14"/>
+      <c r="E16" s="30" t="s">
+        <v>36</v>
       </c>
       <c r="F16" s="14"/>
-      <c r="G16" s="15" t="s">
-        <v>62</v>
+      <c r="G16" s="31" t="s">
+        <v>52</v>
       </c>
       <c r="H16" s="15"/>
-      <c r="I16" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>86</v>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
@@ -1347,31 +1290,25 @@
         <f>ROW(A17) - ROW($A$10)</f>
         <v>7</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="30" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="14">
         <v>2</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>48</v>
+      <c r="D17" s="14"/>
+      <c r="E17" s="30" t="s">
+        <v>37</v>
       </c>
       <c r="F17" s="14"/>
-      <c r="G17" s="15" t="s">
-        <v>63</v>
+      <c r="G17" s="31" t="s">
+        <v>53</v>
       </c>
       <c r="H17" s="15"/>
-      <c r="I17" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>86</v>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="51" x14ac:dyDescent="0.25">
@@ -1379,29 +1316,25 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="30" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="14">
         <v>2</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>49</v>
+      <c r="D18" s="14"/>
+      <c r="E18" s="30" t="s">
+        <v>38</v>
       </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="31" t="s">
         <v>64</v>
-      </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
@@ -1409,31 +1342,25 @@
         <f>ROW(A19) - ROW($A$10)</f>
         <v>9</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="30" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="14">
         <v>1</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="14">
-        <v>651005136421</v>
+      <c r="D19" s="14"/>
+      <c r="E19" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="F19" s="14"/>
-      <c r="G19" s="15" t="s">
-        <v>65</v>
+      <c r="G19" s="31" t="s">
+        <v>55</v>
       </c>
       <c r="H19" s="15"/>
-      <c r="I19" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>86</v>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
@@ -1441,31 +1368,25 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="30" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="14">
         <v>1</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>50</v>
+      <c r="D20" s="14"/>
+      <c r="E20" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="F20" s="14"/>
-      <c r="G20" s="15" t="s">
-        <v>66</v>
+      <c r="G20" s="31" t="s">
+        <v>56</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>86</v>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
@@ -1473,29 +1394,25 @@
         <f>ROW(A21) - ROW($A$10)</f>
         <v>11</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="14">
         <v>1</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>51</v>
+      <c r="D21" s="14"/>
+      <c r="E21" s="30" t="s">
+        <v>41</v>
       </c>
       <c r="F21" s="14"/>
-      <c r="G21" s="15" t="s">
-        <v>67</v>
+      <c r="G21" s="31" t="s">
+        <v>57</v>
       </c>
       <c r="H21" s="15"/>
-      <c r="I21" s="15" t="s">
-        <v>76</v>
-      </c>
+      <c r="I21" s="15"/>
       <c r="J21" s="15"/>
-      <c r="K21" s="15" t="s">
-        <v>86</v>
+      <c r="K21" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
@@ -1503,31 +1420,25 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="30" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="14">
         <v>1</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>52</v>
+      <c r="D22" s="14"/>
+      <c r="E22" s="30" t="s">
+        <v>42</v>
       </c>
       <c r="F22" s="14"/>
-      <c r="G22" s="15" t="s">
-        <v>68</v>
+      <c r="G22" s="31" t="s">
+        <v>58</v>
       </c>
       <c r="H22" s="15"/>
-      <c r="I22" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>86</v>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
@@ -1535,31 +1446,25 @@
         <f>ROW(A23) - ROW($A$10)</f>
         <v>13</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="30" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="14">
         <v>1</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>53</v>
+      <c r="D23" s="14"/>
+      <c r="E23" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="F23" s="14"/>
-      <c r="G23" s="15" t="s">
-        <v>69</v>
+      <c r="G23" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="H23" s="15"/>
-      <c r="I23" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K23" s="15" t="s">
-        <v>86</v>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
@@ -1567,29 +1472,25 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="30" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="14">
         <v>1</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>54</v>
+      <c r="D24" s="14"/>
+      <c r="E24" s="30" t="s">
+        <v>44</v>
       </c>
       <c r="F24" s="14"/>
-      <c r="G24" s="15" t="s">
-        <v>70</v>
+      <c r="G24" s="31" t="s">
+        <v>60</v>
       </c>
       <c r="H24" s="15"/>
-      <c r="I24" s="15" t="s">
-        <v>82</v>
-      </c>
+      <c r="I24" s="15"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="15" t="s">
-        <v>86</v>
+      <c r="K24" s="31" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1728,36 +1629,66 @@
     <mergeCell ref="E5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="K11:K12">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>"Not Fitted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>"Not Fitted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"Not Fitted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>"Not Fitted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>"Not Fitted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"Not Fitted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13:K14">
+  <conditionalFormatting sqref="K19">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K15:K16">
+  <conditionalFormatting sqref="K20">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17:K18">
+  <conditionalFormatting sqref="K21">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K20">
+  <conditionalFormatting sqref="K22">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
+  <conditionalFormatting sqref="K23">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K23:K24">
+  <conditionalFormatting sqref="K24">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Not Fitted"</formula>
     </cfRule>

</xml_diff>